<commit_message>
Update data for 2021
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2021.xlsx
+++ b/data/GroupingsOBSQuestions2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gnat/Workspace/ibp-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F992612B-794F-A643-B6D3-E89F73E92D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2936BF62-9870-274E-AFC2-8B2F69CB85E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23800" windowHeight="13180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8560" yWindow="7980" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionsGroups 2015" sheetId="1" state="hidden" r:id="rId1"/>
@@ -134,6 +134,9 @@
     <t>17-18, 47-52, 55-56, 92-94</t>
   </si>
   <si>
+    <t>Groupings for the OBS Questions (based on the 2019 and 2017 Questionnaire)</t>
+  </si>
+  <si>
     <t>1-102, 143-149</t>
   </si>
   <si>
@@ -555,9 +558,6 @@
   </si>
   <si>
     <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>Groupings for the OBS Questions (based on the 2021 and 2019 Questionnaire)</t>
   </si>
 </sst>
 </file>
@@ -1252,9 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1266,7 +1264,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
@@ -1284,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1295,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1303,10 +1301,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,10 +1312,10 @@
         <v>3.1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,10 +1323,10 @@
         <v>3.2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1348,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1359,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1370,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1392,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1405,7 +1403,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1416,7 +1414,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1427,7 +1425,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1492,8 +1490,8 @@
   </sheetPr>
   <dimension ref="A1:AMI39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1509,7 +1507,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8"/>
@@ -1517,451 +1515,451 @@
     <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D20" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D21" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G22" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G23" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G24" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G25" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G26" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G27" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G28" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G29" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G30" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G31" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G32" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G38" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G39" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>